<commit_message>
fixed name of Mauritius
</commit_message>
<xml_diff>
--- a/CountryReconciler/reconciler/files/country_list.xlsx
+++ b/CountryReconciler/reconciler/files/country_list.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\CountryReconciler\reconciler\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-435" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="-432" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="BL260" authorId="0">
+    <comment ref="BL260" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -6666,8 +6671,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="39">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -7642,10 +7647,11 @@
     <cellStyle name="60% - Énfasis4" xfId="178" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="182" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="186" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="152" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="152" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="157" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="159" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="158" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="148" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="151" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="163" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="167" builtinId="33" customBuiltin="1"/>
@@ -7809,7 +7815,6 @@
     <cellStyle name="Texto de advertencia" xfId="160" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="161" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="147" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="148" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="149" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="150" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="162" builtinId="25" customBuiltin="1"/>
@@ -7822,6 +7827,14 @@
       <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -8424,6 +8437,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12694920" cy="12847320"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8470,7 +8531,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8502,9 +8563,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8536,6 +8598,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8711,63 +8774,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C236" sqref="C236"/>
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="6" max="7" width="32.140625" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.28515625" customWidth="1"/>
-    <col min="11" max="11" width="36.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="6" max="7" width="32.109375" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" customWidth="1"/>
+    <col min="10" max="10" width="30.33203125" customWidth="1"/>
+    <col min="11" max="11" width="36.44140625" customWidth="1"/>
+    <col min="12" max="12" width="19.44140625" customWidth="1"/>
     <col min="13" max="13" width="6" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" customWidth="1"/>
-    <col min="21" max="22" width="5.42578125" customWidth="1"/>
-    <col min="23" max="23" width="24.140625" customWidth="1"/>
-    <col min="24" max="24" width="22.85546875" customWidth="1"/>
-    <col min="25" max="25" width="4.140625" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" customWidth="1"/>
-    <col min="27" max="27" width="9.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.44140625" customWidth="1"/>
+    <col min="19" max="19" width="9.44140625" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" customWidth="1"/>
+    <col min="21" max="22" width="5.44140625" customWidth="1"/>
+    <col min="23" max="23" width="24.109375" customWidth="1"/>
+    <col min="24" max="24" width="22.88671875" customWidth="1"/>
+    <col min="25" max="25" width="4.109375" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" customWidth="1"/>
+    <col min="27" max="27" width="9.88671875" customWidth="1"/>
     <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" customWidth="1"/>
-    <col min="30" max="30" width="11.140625" customWidth="1"/>
-    <col min="31" max="31" width="10.42578125" customWidth="1"/>
-    <col min="32" max="32" width="10.7109375" customWidth="1"/>
-    <col min="33" max="33" width="9.42578125" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" customWidth="1"/>
-    <col min="36" max="36" width="8.7109375" customWidth="1"/>
-    <col min="37" max="37" width="9.42578125" customWidth="1"/>
-    <col min="38" max="39" width="22.140625" customWidth="1"/>
-    <col min="40" max="40" width="23.28515625" customWidth="1"/>
-    <col min="41" max="41" width="23.140625" customWidth="1"/>
-    <col min="42" max="42" width="13.28515625" customWidth="1"/>
-    <col min="43" max="43" width="10.42578125" customWidth="1"/>
-    <col min="44" max="44" width="8.85546875" customWidth="1"/>
-    <col min="45" max="45" width="11.42578125" customWidth="1"/>
-    <col min="46" max="46" width="11.85546875" customWidth="1"/>
-    <col min="47" max="47" width="15.28515625" customWidth="1"/>
-    <col min="48" max="48" width="14.42578125" customWidth="1"/>
+    <col min="29" max="29" width="10.44140625" customWidth="1"/>
+    <col min="30" max="30" width="11.109375" customWidth="1"/>
+    <col min="31" max="31" width="10.44140625" customWidth="1"/>
+    <col min="32" max="32" width="10.6640625" customWidth="1"/>
+    <col min="33" max="33" width="9.44140625" customWidth="1"/>
+    <col min="34" max="34" width="11.44140625" customWidth="1"/>
+    <col min="35" max="35" width="14.44140625" customWidth="1"/>
+    <col min="36" max="36" width="8.6640625" customWidth="1"/>
+    <col min="37" max="37" width="9.44140625" customWidth="1"/>
+    <col min="38" max="39" width="22.109375" customWidth="1"/>
+    <col min="40" max="40" width="23.33203125" customWidth="1"/>
+    <col min="41" max="41" width="23.109375" customWidth="1"/>
+    <col min="42" max="42" width="13.33203125" customWidth="1"/>
+    <col min="43" max="43" width="10.44140625" customWidth="1"/>
+    <col min="44" max="44" width="8.88671875" customWidth="1"/>
+    <col min="45" max="45" width="11.44140625" customWidth="1"/>
+    <col min="46" max="46" width="11.88671875" customWidth="1"/>
+    <col min="47" max="47" width="15.33203125" customWidth="1"/>
+    <col min="48" max="48" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="12.75" customHeight="1">
+    <row r="1" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -8913,7 +8976,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="2" spans="1:48" ht="12.75" customHeight="1">
+    <row r="2" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>45</v>
       </c>
@@ -9057,7 +9120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:48" ht="12.75" customHeight="1">
+    <row r="3" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>57</v>
       </c>
@@ -9201,7 +9264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:48" ht="12.75" customHeight="1">
+    <row r="4" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>72</v>
       </c>
@@ -9345,7 +9408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:48" ht="12.75" customHeight="1">
+    <row r="5" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>84</v>
       </c>
@@ -9489,7 +9552,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:48" ht="12.75" customHeight="1">
+    <row r="6" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>91</v>
       </c>
@@ -9633,7 +9696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:48" ht="12.75" customHeight="1">
+    <row r="7" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>104</v>
       </c>
@@ -9773,7 +9836,7 @@
       </c>
       <c r="AV7" s="22"/>
     </row>
-    <row r="8" spans="1:48" ht="12.75" customHeight="1">
+    <row r="8" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>114</v>
       </c>
@@ -9917,7 +9980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:48" ht="12.75" customHeight="1">
+    <row r="9" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>124</v>
       </c>
@@ -10061,7 +10124,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="12.75" customHeight="1">
+    <row r="10" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>136</v>
       </c>
@@ -10205,7 +10268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="12.75" customHeight="1">
+    <row r="11" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>147</v>
       </c>
@@ -10349,7 +10412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:48" ht="12.75" customHeight="1">
+    <row r="12" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>156</v>
       </c>
@@ -10493,7 +10556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:48" ht="12.75" customHeight="1">
+    <row r="13" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>168</v>
       </c>
@@ -10635,7 +10698,7 @@
       </c>
       <c r="AV13" s="12"/>
     </row>
-    <row r="14" spans="1:48" ht="12.75" customHeight="1">
+    <row r="14" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>177</v>
       </c>
@@ -10775,7 +10838,7 @@
       </c>
       <c r="AV14" s="22"/>
     </row>
-    <row r="15" spans="1:48" ht="12.75" customHeight="1">
+    <row r="15" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>184</v>
       </c>
@@ -10915,7 +10978,7 @@
       </c>
       <c r="AV15" s="22"/>
     </row>
-    <row r="16" spans="1:48" ht="12.75" customHeight="1">
+    <row r="16" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>191</v>
       </c>
@@ -11059,7 +11122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:48" ht="12.75" customHeight="1">
+    <row r="17" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>177</v>
       </c>
@@ -11203,7 +11266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:48" ht="12.75" customHeight="1">
+    <row r="18" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>202</v>
       </c>
@@ -11347,7 +11410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:48" ht="12.75" customHeight="1">
+    <row r="19" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>213</v>
       </c>
@@ -11491,7 +11554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:48" ht="12.75" customHeight="1">
+    <row r="20" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>223</v>
       </c>
@@ -11635,7 +11698,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:48" ht="12.75" customHeight="1">
+    <row r="21" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>232</v>
       </c>
@@ -11779,7 +11842,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="22" spans="1:48" ht="12.75" customHeight="1">
+    <row r="22" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>243</v>
       </c>
@@ -11923,7 +11986,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:48" ht="12.75" customHeight="1">
+    <row r="23" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>252</v>
       </c>
@@ -12067,7 +12130,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="24" spans="1:48" ht="12.75" customHeight="1">
+    <row r="24" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>258</v>
       </c>
@@ -12211,7 +12274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:48" ht="12.75" customHeight="1">
+    <row r="25" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>266</v>
       </c>
@@ -12355,7 +12418,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:48" ht="12.75" customHeight="1">
+    <row r="26" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>276</v>
       </c>
@@ -12499,7 +12562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:48" ht="12.75" customHeight="1">
+    <row r="27" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>286</v>
       </c>
@@ -12643,7 +12706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:48" ht="12.75" customHeight="1">
+    <row r="28" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>295</v>
       </c>
@@ -12787,7 +12850,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:48">
+    <row r="29" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>184</v>
       </c>
@@ -12929,7 +12992,7 @@
       </c>
       <c r="AV29" s="11"/>
     </row>
-    <row r="30" spans="1:48">
+    <row r="30" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>314</v>
       </c>
@@ -13073,7 +13136,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:48">
+    <row r="31" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>324</v>
       </c>
@@ -13217,7 +13280,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:48">
+    <row r="32" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>84</v>
       </c>
@@ -13361,7 +13424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:48" ht="25.5">
+    <row r="33" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>340</v>
       </c>
@@ -13505,7 +13568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:48" ht="25.5">
+    <row r="34" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>348</v>
       </c>
@@ -13649,7 +13712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:48">
+    <row r="35" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>358</v>
       </c>
@@ -13793,7 +13856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:48">
+    <row r="36" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>365</v>
       </c>
@@ -13937,7 +14000,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:48">
+    <row r="37" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>373</v>
       </c>
@@ -14081,7 +14144,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:48">
+    <row r="38" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>382</v>
       </c>
@@ -14225,7 +14288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:48">
+    <row r="39" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>391</v>
       </c>
@@ -14369,7 +14432,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:48">
+    <row r="40" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>401</v>
       </c>
@@ -14513,7 +14576,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:48">
+    <row r="41" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>410</v>
       </c>
@@ -14657,7 +14720,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:48">
+    <row r="42" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>420</v>
       </c>
@@ -14801,7 +14864,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:48">
+    <row r="43" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>428</v>
       </c>
@@ -14945,7 +15008,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="44" spans="1:48">
+    <row r="44" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>437</v>
       </c>
@@ -15089,7 +15152,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:48">
+    <row r="45" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>447</v>
       </c>
@@ -15233,7 +15296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:48" ht="25.5">
+    <row r="46" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>457</v>
       </c>
@@ -15377,7 +15440,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:48">
+    <row r="47" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>470</v>
       </c>
@@ -15521,7 +15584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:48">
+    <row r="48" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>479</v>
       </c>
@@ -15665,7 +15728,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:48">
+    <row r="49" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>490</v>
       </c>
@@ -15809,7 +15872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:48">
+    <row r="50" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>499</v>
       </c>
@@ -15953,7 +16016,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:48">
+    <row r="51" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>509</v>
       </c>
@@ -16097,7 +16160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:48">
+    <row r="52" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>519</v>
       </c>
@@ -16241,7 +16304,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:48">
+    <row r="53" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>527</v>
       </c>
@@ -16385,7 +16448,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:48">
+    <row r="54" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>45</v>
       </c>
@@ -16527,7 +16590,7 @@
       </c>
       <c r="AV54" s="11"/>
     </row>
-    <row r="55" spans="1:48">
+    <row r="55" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>84</v>
       </c>
@@ -16671,7 +16734,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:48" ht="25.5">
+    <row r="56" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
         <v>548</v>
       </c>
@@ -16811,7 +16874,7 @@
       </c>
       <c r="AV56" s="22"/>
     </row>
-    <row r="57" spans="1:48">
+    <row r="57" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>552</v>
       </c>
@@ -16955,7 +17018,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:48">
+    <row r="58" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>561</v>
       </c>
@@ -17099,7 +17162,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:48" ht="25.5">
+    <row r="59" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>571</v>
       </c>
@@ -17243,7 +17306,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:48">
+    <row r="60" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>582</v>
       </c>
@@ -17387,7 +17450,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:48">
+    <row r="61" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>590</v>
       </c>
@@ -17531,7 +17594,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:48">
+    <row r="62" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>599</v>
       </c>
@@ -17675,7 +17738,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:48">
+    <row r="63" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>609</v>
       </c>
@@ -17819,7 +17882,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:48" ht="25.5">
+    <row r="64" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>619</v>
       </c>
@@ -17963,7 +18026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:48">
+    <row r="65" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>630</v>
       </c>
@@ -18107,7 +18170,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:48">
+    <row r="66" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>639</v>
       </c>
@@ -18251,7 +18314,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:48">
+    <row r="67" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>648</v>
       </c>
@@ -18395,7 +18458,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="68" spans="1:48">
+    <row r="68" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>655</v>
       </c>
@@ -18539,7 +18602,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:48">
+    <row r="69" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>666</v>
       </c>
@@ -18683,7 +18746,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="1:48" ht="25.5">
+    <row r="70" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>675</v>
       </c>
@@ -18827,7 +18890,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="71" spans="1:48">
+    <row r="71" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>104</v>
       </c>
@@ -18971,7 +19034,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:48">
+    <row r="72" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>694</v>
       </c>
@@ -19115,7 +19178,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:48" ht="25.5">
+    <row r="73" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>84</v>
       </c>
@@ -19259,7 +19322,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:48">
+    <row r="74" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>184</v>
       </c>
@@ -19403,7 +19466,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:48">
+    <row r="75" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>599</v>
       </c>
@@ -19547,7 +19610,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:48" ht="25.5">
+    <row r="76" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>732</v>
       </c>
@@ -19691,7 +19754,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="1:48">
+    <row r="77" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>742</v>
       </c>
@@ -19835,7 +19898,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:48" ht="25.5">
+    <row r="78" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>84</v>
       </c>
@@ -19979,7 +20042,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="79" spans="1:48">
+    <row r="79" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>759</v>
       </c>
@@ -20123,7 +20186,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:48">
+    <row r="80" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
         <v>84</v>
       </c>
@@ -20263,7 +20326,7 @@
       </c>
       <c r="AV80" s="22"/>
     </row>
-    <row r="81" spans="1:48">
+    <row r="81" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>773</v>
       </c>
@@ -20407,7 +20470,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:48">
+    <row r="82" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="27"/>
       <c r="B82" s="27"/>
       <c r="C82" s="27"/>
@@ -20475,7 +20538,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:48">
+    <row r="83" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>782</v>
       </c>
@@ -20619,7 +20682,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:48">
+    <row r="84" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="27"/>
       <c r="B84" s="27"/>
       <c r="C84" s="27"/>
@@ -20687,7 +20750,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="1:48">
+    <row r="85" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>795</v>
       </c>
@@ -20831,7 +20894,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:48">
+    <row r="86" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>804</v>
       </c>
@@ -20975,7 +21038,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:48" ht="25.5">
+    <row r="87" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>814</v>
       </c>
@@ -21119,7 +21182,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="88" spans="1:48">
+    <row r="88" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>824</v>
       </c>
@@ -21263,7 +21326,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:48">
+    <row r="89" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>833</v>
       </c>
@@ -21407,7 +21470,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:48">
+    <row r="90" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>599</v>
       </c>
@@ -21549,7 +21612,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:48">
+    <row r="91" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>846</v>
       </c>
@@ -21693,7 +21756,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:48">
+    <row r="92" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>156</v>
       </c>
@@ -21837,7 +21900,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:48">
+    <row r="93" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="34"/>
       <c r="B93" s="34"/>
       <c r="C93" s="34"/>
@@ -21905,7 +21968,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:48">
+    <row r="94" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>863</v>
       </c>
@@ -22049,7 +22112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:48" ht="38.25">
+    <row r="95" spans="1:48" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A95" s="19" t="s">
         <v>428</v>
       </c>
@@ -22189,7 +22252,7 @@
       </c>
       <c r="AV95" s="22"/>
     </row>
-    <row r="96" spans="1:48">
+    <row r="96" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="19" t="s">
         <v>177</v>
       </c>
@@ -22329,7 +22392,7 @@
       </c>
       <c r="AV96" s="22"/>
     </row>
-    <row r="97" spans="1:48">
+    <row r="97" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>883</v>
       </c>
@@ -22473,7 +22536,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:48">
+    <row r="98" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>891</v>
       </c>
@@ -22617,7 +22680,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:48">
+    <row r="99" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>901</v>
       </c>
@@ -22761,7 +22824,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="1:48">
+    <row r="100" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>910</v>
       </c>
@@ -22905,7 +22968,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:48">
+    <row r="101" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>918</v>
       </c>
@@ -23049,7 +23112,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:48">
+    <row r="102" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="19" t="s">
         <v>84</v>
       </c>
@@ -23191,7 +23254,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="103" spans="1:48">
+    <row r="103" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>935</v>
       </c>
@@ -23335,7 +23398,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:48">
+    <row r="104" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="19" t="s">
         <v>177</v>
       </c>
@@ -23475,7 +23538,7 @@
       </c>
       <c r="AV104" s="22"/>
     </row>
-    <row r="105" spans="1:48" ht="25.5">
+    <row r="105" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A105" s="19" t="s">
         <v>84</v>
       </c>
@@ -23615,7 +23678,7 @@
       </c>
       <c r="AV105" s="22"/>
     </row>
-    <row r="106" spans="1:48">
+    <row r="106" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>951</v>
       </c>
@@ -23759,7 +23822,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:48">
+    <row r="107" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>959</v>
       </c>
@@ -23903,7 +23966,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:48">
+    <row r="108" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>967</v>
       </c>
@@ -24047,7 +24110,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="109" spans="1:48">
+    <row r="109" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>975</v>
       </c>
@@ -24191,7 +24254,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="110" spans="1:48">
+    <row r="110" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>984</v>
       </c>
@@ -24335,7 +24398,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:48">
+    <row r="111" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>993</v>
       </c>
@@ -24479,7 +24542,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:48">
+    <row r="112" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>1003</v>
       </c>
@@ -24623,7 +24686,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:48">
+    <row r="113" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="19" t="s">
         <v>84</v>
       </c>
@@ -24763,7 +24826,7 @@
       </c>
       <c r="AV113" s="22"/>
     </row>
-    <row r="114" spans="1:48" ht="25.5">
+    <row r="114" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>1016</v>
       </c>
@@ -24907,7 +24970,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:48">
+    <row r="115" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>1026</v>
       </c>
@@ -25051,7 +25114,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="116" spans="1:48">
+    <row r="116" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="19" t="s">
         <v>1034</v>
       </c>
@@ -25191,7 +25254,7 @@
       </c>
       <c r="AV116" s="22"/>
     </row>
-    <row r="117" spans="1:48">
+    <row r="117" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>1039</v>
       </c>
@@ -25335,7 +25398,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="118" spans="1:48">
+    <row r="118" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>1049</v>
       </c>
@@ -25479,7 +25542,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:48">
+    <row r="119" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>1057</v>
       </c>
@@ -25623,7 +25686,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="120" spans="1:48">
+    <row r="120" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>1067</v>
       </c>
@@ -25767,7 +25830,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="121" spans="1:48">
+    <row r="121" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
         <v>1077</v>
       </c>
@@ -25911,7 +25974,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="122" spans="1:48">
+    <row r="122" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
         <v>1085</v>
       </c>
@@ -26055,7 +26118,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="123" spans="1:48">
+    <row r="123" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>1092</v>
       </c>
@@ -26199,7 +26262,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="124" spans="1:48">
+    <row r="124" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="19" t="s">
         <v>1103</v>
       </c>
@@ -26339,7 +26402,7 @@
       </c>
       <c r="AV124" s="22"/>
     </row>
-    <row r="125" spans="1:48">
+    <row r="125" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>1110</v>
       </c>
@@ -26483,7 +26546,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="126" spans="1:48" ht="25.5">
+    <row r="126" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
         <v>1119</v>
       </c>
@@ -26627,7 +26690,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:48">
+    <row r="127" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
         <v>1128</v>
       </c>
@@ -26771,7 +26834,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="128" spans="1:48">
+    <row r="128" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>1138</v>
       </c>
@@ -26915,7 +26978,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="129" spans="1:48">
+    <row r="129" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>1146</v>
       </c>
@@ -27059,7 +27122,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="130" spans="1:48">
+    <row r="130" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>1152</v>
       </c>
@@ -27203,7 +27266,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="131" spans="1:48">
+    <row r="131" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>1159</v>
       </c>
@@ -27347,7 +27410,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="132" spans="1:48" ht="25.5">
+    <row r="132" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>1168</v>
       </c>
@@ -27491,7 +27554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="133" spans="1:48">
+    <row r="133" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>1176</v>
       </c>
@@ -27635,7 +27698,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="134" spans="1:48">
+    <row r="134" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>1184</v>
       </c>
@@ -27779,7 +27842,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="135" spans="1:48">
+    <row r="135" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
         <v>1194</v>
       </c>
@@ -27923,7 +27986,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="136" spans="1:48">
+    <row r="136" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>1204</v>
       </c>
@@ -28067,7 +28130,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="137" spans="1:48">
+    <row r="137" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="19" t="s">
         <v>428</v>
       </c>
@@ -28207,7 +28270,7 @@
       </c>
       <c r="AV137" s="22"/>
     </row>
-    <row r="138" spans="1:48" s="12" customFormat="1">
+    <row r="138" spans="1:48" s="12" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>184</v>
       </c>
@@ -28349,7 +28412,7 @@
       </c>
       <c r="AV138" s="11"/>
     </row>
-    <row r="139" spans="1:48">
+    <row r="139" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>1229</v>
       </c>
@@ -28493,7 +28556,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="140" spans="1:48">
+    <row r="140" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
         <v>1239</v>
       </c>
@@ -28637,7 +28700,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="141" spans="1:48">
+    <row r="141" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>1248</v>
       </c>
@@ -28781,7 +28844,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="142" spans="1:48">
+    <row r="142" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
         <v>1256</v>
       </c>
@@ -28925,7 +28988,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="143" spans="1:48">
+    <row r="143" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>1264</v>
       </c>
@@ -29069,7 +29132,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="144" spans="1:48">
+    <row r="144" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>1274</v>
       </c>
@@ -29213,7 +29276,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="145" spans="1:48" ht="25.5">
+    <row r="145" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>1284</v>
       </c>
@@ -29357,7 +29420,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="146" spans="1:48" ht="25.5">
+    <row r="146" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>1294</v>
       </c>
@@ -29501,7 +29564,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="147" spans="1:48">
+    <row r="147" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>1303</v>
       </c>
@@ -29645,7 +29708,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="148" spans="1:48">
+    <row r="148" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>1311</v>
       </c>
@@ -29789,7 +29852,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="149" spans="1:48" ht="25.5">
+    <row r="149" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>1320</v>
       </c>
@@ -29933,7 +29996,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="150" spans="1:48">
+    <row r="150" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
         <v>1328</v>
       </c>
@@ -30077,7 +30140,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="151" spans="1:48">
+    <row r="151" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>1335</v>
       </c>
@@ -30221,7 +30284,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="152" spans="1:48">
+    <row r="152" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="19" t="s">
         <v>156</v>
       </c>
@@ -30363,7 +30426,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="153" spans="1:48">
+    <row r="153" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
         <v>1347</v>
       </c>
@@ -30507,7 +30570,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="154" spans="1:48" ht="25.5">
+    <row r="154" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
         <v>1355</v>
       </c>
@@ -30651,7 +30714,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="155" spans="1:48">
+    <row r="155" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="13" t="s">
         <v>84</v>
       </c>
@@ -30795,7 +30858,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="156" spans="1:48">
+    <row r="156" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="27"/>
       <c r="B156" s="27"/>
       <c r="C156" s="27"/>
@@ -30863,7 +30926,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="157" spans="1:48">
+    <row r="157" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
         <v>1373</v>
       </c>
@@ -30879,8 +30942,8 @@
       <c r="E157" s="13" t="s">
         <v>1374</v>
       </c>
-      <c r="F157" s="18" t="s">
-        <v>1370</v>
+      <c r="F157" s="12" t="s">
+        <v>1373</v>
       </c>
       <c r="G157" s="12" t="s">
         <v>1373</v>
@@ -31007,7 +31070,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="158" spans="1:48">
+    <row r="158" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>1382</v>
       </c>
@@ -31151,7 +31214,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="159" spans="1:48">
+    <row r="159" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>1390</v>
       </c>
@@ -31295,7 +31358,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="160" spans="1:48">
+    <row r="160" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
         <v>1398</v>
       </c>
@@ -31439,7 +31502,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="161" spans="1:48">
+    <row r="161" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
         <v>184</v>
       </c>
@@ -31583,7 +31646,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="162" spans="1:48">
+    <row r="162" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
         <v>1415</v>
       </c>
@@ -31727,7 +31790,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="163" spans="1:48">
+    <row r="163" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="19" t="s">
         <v>177</v>
       </c>
@@ -31869,7 +31932,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:48">
+    <row r="164" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
         <v>1428</v>
       </c>
@@ -32013,7 +32076,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="165" spans="1:48">
+    <row r="165" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
         <v>1436</v>
       </c>
@@ -32157,7 +32220,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="166" spans="1:48">
+    <row r="166" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
         <v>479</v>
       </c>
@@ -32301,7 +32364,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="167" spans="1:48">
+    <row r="167" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
         <v>45</v>
       </c>
@@ -32445,7 +32508,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="168" spans="1:48">
+    <row r="168" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
         <v>1461</v>
       </c>
@@ -32589,7 +32652,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="169" spans="1:48" ht="25.5">
+    <row r="169" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A169" s="13" t="s">
         <v>1472</v>
       </c>
@@ -32733,7 +32796,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="170" spans="1:48">
+    <row r="170" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
         <v>1480</v>
       </c>
@@ -32877,7 +32940,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="171" spans="1:48">
+    <row r="171" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
         <v>479</v>
       </c>
@@ -33021,7 +33084,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="172" spans="1:48">
+    <row r="172" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>1494</v>
       </c>
@@ -33165,7 +33228,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="173" spans="1:48" ht="25.5">
+    <row r="173" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
         <v>1502</v>
       </c>
@@ -33309,7 +33372,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="174" spans="1:48">
+    <row r="174" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
         <v>1511</v>
       </c>
@@ -33453,7 +33516,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="175" spans="1:48">
+    <row r="175" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="19" t="s">
         <v>84</v>
       </c>
@@ -33595,7 +33658,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="176" spans="1:48">
+    <row r="176" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
         <v>1525</v>
       </c>
@@ -33739,7 +33802,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="177" spans="1:48">
+    <row r="177" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
         <v>1534</v>
       </c>
@@ -33883,7 +33946,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="178" spans="1:48">
+    <row r="178" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
         <v>1543</v>
       </c>
@@ -34027,7 +34090,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="179" spans="1:48">
+    <row r="179" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
         <v>1551</v>
       </c>
@@ -34171,7 +34234,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="180" spans="1:48">
+    <row r="180" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
         <v>1559</v>
       </c>
@@ -34315,7 +34378,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="181" spans="1:48" ht="25.5">
+    <row r="181" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
         <v>156</v>
       </c>
@@ -34459,7 +34522,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="182" spans="1:48" ht="25.5">
+    <row r="182" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A182" s="13" t="s">
         <v>1578</v>
       </c>
@@ -34603,7 +34666,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="183" spans="1:48">
+    <row r="183" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="13" t="s">
         <v>1589</v>
       </c>
@@ -34747,7 +34810,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="184" spans="1:48">
+    <row r="184" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="13" t="s">
         <v>1598</v>
       </c>
@@ -34891,7 +34954,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="185" spans="1:48">
+    <row r="185" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="19" t="s">
         <v>984</v>
       </c>
@@ -35031,7 +35094,7 @@
       </c>
       <c r="AV185" s="22"/>
     </row>
-    <row r="186" spans="1:48">
+    <row r="186" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="13" t="s">
         <v>184</v>
       </c>
@@ -35175,7 +35238,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="187" spans="1:48">
+    <row r="187" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="13" t="s">
         <v>1624</v>
       </c>
@@ -35319,7 +35382,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="188" spans="1:48">
+    <row r="188" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="27"/>
       <c r="B188" s="27"/>
       <c r="C188" s="27"/>
@@ -35387,7 +35450,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="189" spans="1:48">
+    <row r="189" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="13" t="s">
         <v>1635</v>
       </c>
@@ -35531,7 +35594,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="190" spans="1:48">
+    <row r="190" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="13" t="s">
         <v>1645</v>
       </c>
@@ -35675,7 +35738,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="191" spans="1:48">
+    <row r="191" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="13" t="s">
         <v>1656</v>
       </c>
@@ -35819,7 +35882,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="192" spans="1:48">
+    <row r="192" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="19" t="s">
         <v>1664</v>
       </c>
@@ -35961,7 +36024,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="193" spans="1:48">
+    <row r="193" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="13" t="s">
         <v>1671</v>
       </c>
@@ -36105,7 +36168,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="194" spans="1:48">
+    <row r="194" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
         <v>1681</v>
       </c>
@@ -36249,7 +36312,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="195" spans="1:48">
+    <row r="195" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="13" t="s">
         <v>1690</v>
       </c>
@@ -36393,7 +36456,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="196" spans="1:48">
+    <row r="196" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="13" t="s">
         <v>1699</v>
       </c>
@@ -36537,7 +36600,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="197" spans="1:48" ht="25.5">
+    <row r="197" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A197" s="19" t="s">
         <v>84</v>
       </c>
@@ -36677,7 +36740,7 @@
       </c>
       <c r="AV197" s="22"/>
     </row>
-    <row r="198" spans="1:48" ht="25.5">
+    <row r="198" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A198" s="13" t="s">
         <v>84</v>
       </c>
@@ -36821,7 +36884,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="199" spans="1:48">
+    <row r="199" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="13" t="s">
         <v>1721</v>
       </c>
@@ -36965,7 +37028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:48">
+    <row r="200" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="13" t="s">
         <v>1730</v>
       </c>
@@ -37109,7 +37172,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="201" spans="1:48">
+    <row r="201" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="13" t="s">
         <v>1738</v>
       </c>
@@ -37253,7 +37316,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="202" spans="1:48">
+    <row r="202" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="13" t="s">
         <v>1746</v>
       </c>
@@ -37397,7 +37460,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="203" spans="1:48">
+    <row r="203" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="19" t="s">
         <v>1756</v>
       </c>
@@ -37537,7 +37600,7 @@
       </c>
       <c r="AV203" s="22"/>
     </row>
-    <row r="204" spans="1:48">
+    <row r="204" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="13" t="s">
         <v>1760</v>
       </c>
@@ -37681,7 +37744,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="205" spans="1:48">
+    <row r="205" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="13" t="s">
         <v>184</v>
       </c>
@@ -37825,7 +37888,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="206" spans="1:48">
+    <row r="206" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A206" s="13" t="s">
         <v>1775</v>
       </c>
@@ -37969,7 +38032,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="207" spans="1:48">
+    <row r="207" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="14" t="s">
         <v>1785</v>
       </c>
@@ -38111,7 +38174,7 @@
       </c>
       <c r="AV207" s="40"/>
     </row>
-    <row r="208" spans="1:48" ht="25.5">
+    <row r="208" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A208" s="13" t="s">
         <v>1796</v>
       </c>
@@ -38255,7 +38318,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="209" spans="1:48">
+    <row r="209" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="13" t="s">
         <v>1807</v>
       </c>
@@ -38399,7 +38462,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="1:48">
+    <row r="210" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A210" s="13" t="s">
         <v>1815</v>
       </c>
@@ -38543,7 +38606,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="211" spans="1:48">
+    <row r="211" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A211" s="13" t="s">
         <v>1825</v>
       </c>
@@ -38687,7 +38750,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="212" spans="1:48">
+    <row r="212" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="13" t="s">
         <v>1836</v>
       </c>
@@ -38831,7 +38894,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="213" spans="1:48">
+    <row r="213" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A213" s="13" t="s">
         <v>1847</v>
       </c>
@@ -38975,7 +39038,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="214" spans="1:48" ht="25.5">
+    <row r="214" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
         <v>45</v>
       </c>
@@ -39117,7 +39180,7 @@
       </c>
       <c r="AV214" s="11"/>
     </row>
-    <row r="215" spans="1:48">
+    <row r="215" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A215" s="13" t="s">
         <v>1864</v>
       </c>
@@ -39261,7 +39324,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="216" spans="1:48">
+    <row r="216" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="13" t="s">
         <v>1872</v>
       </c>
@@ -39405,7 +39468,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="217" spans="1:48">
+    <row r="217" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A217" s="13" t="s">
         <v>84</v>
       </c>
@@ -39549,7 +39612,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="218" spans="1:48">
+    <row r="218" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="13" t="s">
         <v>1889</v>
       </c>
@@ -39693,7 +39756,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="219" spans="1:48">
+    <row r="219" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="13" t="s">
         <v>1897</v>
       </c>
@@ -39837,7 +39900,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="1:48">
+    <row r="220" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A220" s="13" t="s">
         <v>1904</v>
       </c>
@@ -39981,7 +40044,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="221" spans="1:48">
+    <row r="221" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A221" s="13" t="s">
         <v>1914</v>
       </c>
@@ -40125,7 +40188,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="222" spans="1:48" s="52" customFormat="1">
+    <row r="222" spans="1:48" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A222" s="46" t="s">
         <v>479</v>
       </c>
@@ -40269,7 +40332,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="223" spans="1:48">
+    <row r="223" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A223" s="13" t="s">
         <v>1927</v>
       </c>
@@ -40413,7 +40476,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="224" spans="1:48" ht="25.5">
+    <row r="224" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A224" s="13" t="s">
         <v>1935</v>
       </c>
@@ -40557,7 +40620,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="225" spans="1:48">
+    <row r="225" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A225" s="13" t="s">
         <v>1946</v>
       </c>
@@ -40701,7 +40764,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="226" spans="1:48" ht="25.5">
+    <row r="226" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A226" s="13" t="s">
         <v>1954</v>
       </c>
@@ -40845,7 +40908,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="227" spans="1:48">
+    <row r="227" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A227" s="13" t="s">
         <v>1964</v>
       </c>
@@ -40989,7 +41052,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="228" spans="1:48">
+    <row r="228" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A228" s="13" t="s">
         <v>1974</v>
       </c>
@@ -41133,7 +41196,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="229" spans="1:48" s="52" customFormat="1">
+    <row r="229" spans="1:48" s="52" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A229" s="46" t="s">
         <v>1987</v>
       </c>
@@ -41277,7 +41340,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="1:48" s="3" customFormat="1">
+    <row r="230" spans="1:48" s="3" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A230" s="47" t="s">
         <v>1984</v>
       </c>
@@ -41416,7 +41479,7 @@
       </c>
       <c r="AV230" s="22"/>
     </row>
-    <row r="231" spans="1:48">
+    <row r="231" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A231" s="13" t="s">
         <v>1990</v>
       </c>
@@ -41560,7 +41623,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="232" spans="1:48">
+    <row r="232" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
         <v>2001</v>
       </c>
@@ -41704,7 +41767,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="233" spans="1:48">
+    <row r="233" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A233" s="13" t="s">
         <v>2010</v>
       </c>
@@ -41848,7 +41911,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="234" spans="1:48" ht="25.5">
+    <row r="234" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A234" s="13" t="s">
         <v>2017</v>
       </c>
@@ -41992,7 +42055,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="235" spans="1:48">
+    <row r="235" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A235" s="13" t="s">
         <v>156</v>
       </c>
@@ -42136,7 +42199,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="236" spans="1:48">
+    <row r="236" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A236" s="13" t="s">
         <v>2035</v>
       </c>
@@ -42280,7 +42343,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:48">
+    <row r="237" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A237" s="13" t="s">
         <v>2045</v>
       </c>
@@ -42424,7 +42487,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="238" spans="1:48">
+    <row r="238" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A238" s="13" t="s">
         <v>2056</v>
       </c>
@@ -42568,7 +42631,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="239" spans="1:48" ht="25.5">
+    <row r="239" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A239" s="13" t="s">
         <v>2063</v>
       </c>
@@ -42712,7 +42775,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="240" spans="1:48">
+    <row r="240" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A240" s="13" t="s">
         <v>84</v>
       </c>
@@ -42856,7 +42919,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:48" ht="25.5">
+    <row r="241" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A241" s="19" t="s">
         <v>156</v>
       </c>
@@ -42998,7 +43061,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:48" ht="25.5">
+    <row r="242" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A242" s="13" t="s">
         <v>2086</v>
       </c>
@@ -43142,7 +43205,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="243" spans="1:48">
+    <row r="243" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A243" s="13" t="s">
         <v>2095</v>
       </c>
@@ -43286,7 +43349,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="244" spans="1:48">
+    <row r="244" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A244" s="13" t="s">
         <v>184</v>
       </c>
@@ -43430,7 +43493,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:48" ht="25.5">
+    <row r="245" spans="1:48" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A245" s="13" t="s">
         <v>2112</v>
       </c>
@@ -43574,7 +43637,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:48">
+    <row r="246" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A246" s="13" t="s">
         <v>2118</v>
       </c>
@@ -43718,7 +43781,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="247" spans="1:48">
+    <row r="247" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A247" s="13" t="s">
         <v>2129</v>
       </c>
@@ -43862,7 +43925,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="248" spans="1:48">
+    <row r="248" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A248" s="13" t="s">
         <v>2139</v>
       </c>
@@ -44006,7 +44069,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="249" spans="1:48">
+    <row r="249" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A249" s="13" t="s">
         <v>2147</v>
       </c>
@@ -44150,7 +44213,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="250" spans="1:48">
+    <row r="250" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A250" s="27"/>
       <c r="B250" s="27"/>
       <c r="C250" s="27"/>
@@ -44216,7 +44279,7 @@
       <c r="AU250" s="27"/>
       <c r="AV250" s="29"/>
     </row>
-    <row r="251" spans="1:48">
+    <row r="251" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
@@ -44264,7 +44327,7 @@
       <c r="AS251" s="2"/>
       <c r="AT251" s="2"/>
     </row>
-    <row r="252" spans="1:48">
+    <row r="252" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -44312,7 +44375,7 @@
       <c r="AS252" s="2"/>
       <c r="AT252" s="2"/>
     </row>
-    <row r="253" spans="1:48">
+    <row r="253" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
@@ -44360,7 +44423,7 @@
       <c r="AS253" s="2"/>
       <c r="AT253" s="2"/>
     </row>
-    <row r="254" spans="1:48">
+    <row r="254" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
@@ -44408,7 +44471,7 @@
       <c r="AS254" s="2"/>
       <c r="AT254" s="2"/>
     </row>
-    <row r="255" spans="1:48">
+    <row r="255" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
@@ -44456,7 +44519,7 @@
       <c r="AS255" s="2"/>
       <c r="AT255" s="2"/>
     </row>
-    <row r="256" spans="1:48">
+    <row r="256" spans="1:48" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
@@ -44504,7 +44567,7 @@
       <c r="AS256" s="2"/>
       <c r="AT256" s="2"/>
     </row>
-    <row r="257" spans="1:64">
+    <row r="257" spans="1:64" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
@@ -44552,7 +44615,7 @@
       <c r="AS257" s="2"/>
       <c r="AT257" s="2"/>
     </row>
-    <row r="258" spans="1:64">
+    <row r="258" spans="1:64" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
@@ -44600,7 +44663,7 @@
       <c r="AS258" s="2"/>
       <c r="AT258" s="2"/>
     </row>
-    <row r="259" spans="1:64">
+    <row r="259" spans="1:64" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
@@ -44648,7 +44711,7 @@
       <c r="AS259" s="2"/>
       <c r="AT259" s="2"/>
     </row>
-    <row r="260" spans="1:64">
+    <row r="260" spans="1:64" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
@@ -44696,7 +44759,7 @@
       <c r="AS260" s="2"/>
       <c r="AT260" s="2"/>
     </row>
-    <row r="261" spans="1:64">
+    <row r="261" spans="1:64" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>

</xml_diff>

<commit_message>
Added iso 2 code for Gibraltar
</commit_message>
<xml_diff>
--- a/CountryReconciler/reconciler/files/country_list.xlsx
+++ b/CountryReconciler/reconciler/files/country_list.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6870" uniqueCount="2208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6871" uniqueCount="2209">
   <si>
     <t>sovereignt,C,254</t>
   </si>
@@ -6666,6 +6666,9 @@
   </si>
   <si>
     <t>772</t>
+  </si>
+  <si>
+    <t>GI</t>
   </si>
 </sst>
 </file>
@@ -7505,7 +7508,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -7627,6 +7630,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="189">
     <cellStyle name="20% - Énfasis1" xfId="164" builtinId="30" customBuiltin="1"/>
@@ -8485,6 +8489,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12694920" cy="12847320"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8778,8 +8830,8 @@
   <dimension ref="A1:BL261"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F157" sqref="F157"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20474,7 +20526,9 @@
       <c r="A82" s="27"/>
       <c r="B82" s="27"/>
       <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
+      <c r="D82" s="55" t="s">
+        <v>2208</v>
+      </c>
       <c r="E82" s="27" t="s">
         <v>780</v>
       </c>

</xml_diff>

<commit_message>
update the country list. Added Kosovo. Added alias for Transparency International
</commit_message>
<xml_diff>
--- a/CountryReconciler/reconciler/files/country_list.xlsx
+++ b/CountryReconciler/reconciler/files/country_list.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9316" uniqueCount="2227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9325" uniqueCount="2230">
   <si>
     <t>sovereignt,C,254</t>
   </si>
@@ -6763,6 +6763,15 @@
   </si>
   <si>
     <t>alternative EN name 1</t>
+  </si>
+  <si>
+    <t>XKX</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>XK</t>
   </si>
 </sst>
 </file>
@@ -7655,7 +7664,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -7823,6 +7832,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="152" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="43" fillId="0" borderId="0" xfId="152" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" xfId="154" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" xfId="154" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -9405,10 +9420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K250"/>
+  <dimension ref="A1:K251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C233" sqref="C233"/>
+    <sheetView tabSelected="1" topLeftCell="A215" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -18168,6 +18183,35 @@
       </c>
       <c r="K250" s="67" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" s="77" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A251" s="77" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="C251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="D251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="E251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="F251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="G251" s="77" t="s">
+        <v>2228</v>
+      </c>
+      <c r="H251" s="77" t="s">
+        <v>2229</v>
+      </c>
+      <c r="K251" s="78" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>